<commit_message>
Fix some issues of conflicting Native status or Name in 04.1.R because I got NAs when doing left_join() between seeded.correct (corrected SpeciesSeeded info) and subplot data. SUNGR.TLE still shows up as NA and not sure why, but manually changed SpeciesSeeded value. Add PlantSource column and write new cleaned subplot data
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/04.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
+++ b/data/data-wrangling-intermediate/04.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40AEC6CF-7E42-4A2D-A06A-850AAA07D1E1}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BA4525C-4E4B-4CBD-9598-B01D4F601BC5}"/>
   <bookViews>
     <workbookView xWindow="41295" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,9 +187,6 @@
     <t>SUNGR.BabbittPJ</t>
   </si>
   <si>
-    <t>Seeded unknown grass (?), BabbittPJ</t>
-  </si>
-  <si>
     <t>UNFO1</t>
   </si>
   <si>
@@ -355,9 +352,6 @@
     <t>SUNGR.TLE</t>
   </si>
   <si>
-    <t>Seeded unknown grass (?), TLE</t>
-  </si>
-  <si>
     <t>UNGR.TLE</t>
   </si>
   <si>
@@ -527,6 +521,12 @@
   </si>
   <si>
     <t>Pectocarya penicillata</t>
+  </si>
+  <si>
+    <t>Seeded unknown grass, BabbittPJ</t>
+  </si>
+  <si>
+    <t>Seeded unknown grass, TLE</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1497,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2009,7 +2009,7 @@
         <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>167</v>
       </c>
       <c r="G16" t="s">
         <v>6</v>
@@ -2035,13 +2035,13 @@
         <v>52</v>
       </c>
       <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
         <v>56</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>57</v>
-      </c>
-      <c r="F17" t="s">
-        <v>58</v>
       </c>
       <c r="G17" t="s">
         <v>6</v>
@@ -2070,10 +2070,10 @@
         <v>35</v>
       </c>
       <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
         <v>59</v>
-      </c>
-      <c r="F18" t="s">
-        <v>60</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
@@ -2102,10 +2102,10 @@
         <v>35</v>
       </c>
       <c r="E19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" t="s">
         <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>60</v>
       </c>
       <c r="G19" t="s">
         <v>6</v>
@@ -2134,13 +2134,13 @@
         <v>44</v>
       </c>
       <c r="E20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s">
         <v>61</v>
       </c>
-      <c r="F20" t="s">
-        <v>62</v>
-      </c>
       <c r="G20" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H20" t="s">
         <v>16</v>
@@ -2154,7 +2154,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
         <v>33</v>
@@ -2163,62 +2163,62 @@
         <v>52</v>
       </c>
       <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" t="s">
         <v>65</v>
-      </c>
-      <c r="G21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" t="s">
-        <v>66</v>
       </c>
       <c r="I21" t="s">
         <v>23</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" t="s">
         <v>65</v>
-      </c>
-      <c r="G22" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" t="s">
-        <v>66</v>
       </c>
       <c r="I22" t="s">
         <v>23</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
@@ -2227,30 +2227,30 @@
         <v>34</v>
       </c>
       <c r="D23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" t="s">
         <v>65</v>
-      </c>
-      <c r="G23" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" t="s">
-        <v>66</v>
       </c>
       <c r="I23" t="s">
         <v>23</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
         <v>33</v>
@@ -2259,13 +2259,13 @@
         <v>34</v>
       </c>
       <c r="D24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
         <v>68</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>69</v>
-      </c>
-      <c r="F24" t="s">
-        <v>70</v>
       </c>
       <c r="G24" t="s">
         <v>6</v>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
@@ -2294,13 +2294,13 @@
         <v>44</v>
       </c>
       <c r="E25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" t="s">
         <v>71</v>
       </c>
-      <c r="F25" t="s">
-        <v>72</v>
-      </c>
       <c r="G25" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H25" t="s">
         <v>16</v>
@@ -2314,7 +2314,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
         <v>33</v>
@@ -2326,13 +2326,13 @@
         <v>44</v>
       </c>
       <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
         <v>71</v>
       </c>
-      <c r="F26" t="s">
-        <v>72</v>
-      </c>
       <c r="G26" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H26" t="s">
         <v>16</v>
@@ -2346,7 +2346,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
         <v>33</v>
@@ -2355,62 +2355,62 @@
         <v>52</v>
       </c>
       <c r="D27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" t="s">
         <v>65</v>
-      </c>
-      <c r="G27" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" t="s">
-        <v>66</v>
       </c>
       <c r="I27" t="s">
         <v>23</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" t="s">
         <v>65</v>
-      </c>
-      <c r="G28" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" t="s">
-        <v>66</v>
       </c>
       <c r="I28" t="s">
         <v>23</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
         <v>33</v>
@@ -2419,30 +2419,30 @@
         <v>34</v>
       </c>
       <c r="D29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" t="s">
         <v>65</v>
-      </c>
-      <c r="G29" t="s">
-        <v>6</v>
-      </c>
-      <c r="H29" t="s">
-        <v>66</v>
       </c>
       <c r="I29" t="s">
         <v>23</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
@@ -2451,13 +2451,13 @@
         <v>34</v>
       </c>
       <c r="D30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="G30" t="s">
         <v>6</v>
@@ -2469,12 +2469,12 @@
         <v>23</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
@@ -2483,13 +2483,13 @@
         <v>52</v>
       </c>
       <c r="D31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" t="s">
         <v>77</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>78</v>
-      </c>
-      <c r="F31" t="s">
-        <v>79</v>
       </c>
       <c r="G31" t="s">
         <v>6</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -2515,13 +2515,13 @@
         <v>34</v>
       </c>
       <c r="D32" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" t="s">
         <v>77</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>78</v>
-      </c>
-      <c r="F32" t="s">
-        <v>79</v>
       </c>
       <c r="G32" t="s">
         <v>6</v>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
         <v>33</v>
@@ -2550,13 +2550,13 @@
         <v>44</v>
       </c>
       <c r="E33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" t="s">
         <v>80</v>
       </c>
-      <c r="F33" t="s">
-        <v>81</v>
-      </c>
       <c r="G33" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H33" t="s">
         <v>16</v>
@@ -2570,7 +2570,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
@@ -2582,13 +2582,13 @@
         <v>44</v>
       </c>
       <c r="E34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" t="s">
         <v>80</v>
       </c>
-      <c r="F34" t="s">
-        <v>81</v>
-      </c>
       <c r="G34" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H34" t="s">
         <v>16</v>
@@ -2602,7 +2602,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
@@ -2614,13 +2614,13 @@
         <v>38</v>
       </c>
       <c r="E35" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" t="s">
         <v>83</v>
       </c>
-      <c r="F35" t="s">
-        <v>84</v>
-      </c>
       <c r="G35" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H35" t="s">
         <v>16</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
         <v>33</v>
@@ -2646,13 +2646,13 @@
         <v>38</v>
       </c>
       <c r="E36" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36" t="s">
         <v>83</v>
       </c>
-      <c r="F36" t="s">
-        <v>84</v>
-      </c>
       <c r="G36" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H36" t="s">
         <v>16</v>
@@ -2666,7 +2666,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
         <v>33</v>
@@ -2678,13 +2678,13 @@
         <v>44</v>
       </c>
       <c r="E37" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" t="s">
         <v>85</v>
       </c>
-      <c r="F37" t="s">
-        <v>86</v>
-      </c>
       <c r="G37" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H37" t="s">
         <v>16</v>
@@ -2698,7 +2698,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
         <v>33</v>
@@ -2710,13 +2710,13 @@
         <v>44</v>
       </c>
       <c r="E38" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" t="s">
         <v>85</v>
       </c>
-      <c r="F38" t="s">
-        <v>86</v>
-      </c>
       <c r="G38" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H38" t="s">
         <v>16</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
         <v>33</v>
@@ -2742,10 +2742,10 @@
         <v>35</v>
       </c>
       <c r="E39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" t="s">
         <v>88</v>
-      </c>
-      <c r="F39" t="s">
-        <v>89</v>
       </c>
       <c r="G39" t="s">
         <v>6</v>
@@ -2762,7 +2762,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
         <v>33</v>
@@ -2774,10 +2774,10 @@
         <v>35</v>
       </c>
       <c r="E40" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" t="s">
         <v>88</v>
-      </c>
-      <c r="F40" t="s">
-        <v>89</v>
       </c>
       <c r="G40" t="s">
         <v>6</v>
@@ -2794,7 +2794,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
         <v>33</v>
@@ -2806,13 +2806,13 @@
         <v>38</v>
       </c>
       <c r="E41" t="s">
+        <v>89</v>
+      </c>
+      <c r="F41" t="s">
         <v>90</v>
       </c>
-      <c r="F41" t="s">
-        <v>91</v>
-      </c>
       <c r="G41" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H41" t="s">
         <v>16</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
         <v>33</v>
@@ -2838,13 +2838,13 @@
         <v>38</v>
       </c>
       <c r="E42" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" t="s">
         <v>90</v>
       </c>
-      <c r="F42" t="s">
-        <v>91</v>
-      </c>
       <c r="G42" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H42" t="s">
         <v>16</v>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B43" t="s">
         <v>33</v>
@@ -2870,10 +2870,10 @@
         <v>41</v>
       </c>
       <c r="E43" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" t="s">
         <v>92</v>
-      </c>
-      <c r="F43" t="s">
-        <v>93</v>
       </c>
       <c r="G43" t="s">
         <v>6</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
         <v>33</v>
@@ -2902,10 +2902,10 @@
         <v>41</v>
       </c>
       <c r="E44" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" t="s">
         <v>92</v>
-      </c>
-      <c r="F44" t="s">
-        <v>93</v>
       </c>
       <c r="G44" t="s">
         <v>6</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
         <v>33</v>
@@ -2934,13 +2934,13 @@
         <v>44</v>
       </c>
       <c r="E45" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45" t="s">
         <v>94</v>
       </c>
-      <c r="F45" t="s">
-        <v>95</v>
-      </c>
       <c r="G45" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H45" t="s">
         <v>16</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
         <v>33</v>
@@ -2966,13 +2966,13 @@
         <v>44</v>
       </c>
       <c r="E46" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" t="s">
         <v>94</v>
       </c>
-      <c r="F46" t="s">
-        <v>95</v>
-      </c>
       <c r="G46" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H46" t="s">
         <v>16</v>
@@ -2986,7 +2986,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
         <v>33</v>
@@ -2995,14 +2995,14 @@
         <v>12</v>
       </c>
       <c r="D47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="G47" t="s">
         <v>6</v>
       </c>
@@ -3013,12 +3013,12 @@
         <v>17</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
         <v>33</v>
@@ -3027,13 +3027,13 @@
         <v>12</v>
       </c>
       <c r="D48" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" t="s">
         <v>100</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>101</v>
-      </c>
-      <c r="F48" t="s">
-        <v>102</v>
       </c>
       <c r="G48" t="s">
         <v>6</v>
@@ -3050,7 +3050,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
         <v>33</v>
@@ -3059,16 +3059,16 @@
         <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E49" t="s">
+        <v>102</v>
+      </c>
+      <c r="F49" t="s">
         <v>103</v>
       </c>
-      <c r="F49" t="s">
-        <v>104</v>
-      </c>
       <c r="G49" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H49" t="s">
         <v>16</v>
@@ -3082,7 +3082,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
         <v>33</v>
@@ -3091,16 +3091,16 @@
         <v>34</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E50" t="s">
+        <v>102</v>
+      </c>
+      <c r="F50" t="s">
         <v>103</v>
       </c>
-      <c r="F50" t="s">
-        <v>104</v>
-      </c>
       <c r="G50" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H50" t="s">
         <v>16</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" t="s">
         <v>33</v>
@@ -3126,13 +3126,13 @@
         <v>44</v>
       </c>
       <c r="E51" t="s">
+        <v>104</v>
+      </c>
+      <c r="F51" t="s">
         <v>105</v>
       </c>
-      <c r="F51" t="s">
-        <v>106</v>
-      </c>
       <c r="G51" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H51" t="s">
         <v>16</v>
@@ -3146,7 +3146,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" t="s">
         <v>33</v>
@@ -3158,13 +3158,13 @@
         <v>44</v>
       </c>
       <c r="E52" t="s">
+        <v>104</v>
+      </c>
+      <c r="F52" t="s">
         <v>105</v>
       </c>
-      <c r="F52" t="s">
-        <v>106</v>
-      </c>
       <c r="G52" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H52" t="s">
         <v>16</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B53" t="s">
         <v>33</v>
@@ -3187,14 +3187,14 @@
         <v>12</v>
       </c>
       <c r="D53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="G53" t="s">
         <v>6</v>
       </c>
@@ -3205,12 +3205,12 @@
         <v>17</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B54" t="s">
         <v>33</v>
@@ -3222,10 +3222,10 @@
         <v>53</v>
       </c>
       <c r="E54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F54" t="s">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="G54" t="s">
         <v>6</v>
@@ -3242,7 +3242,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
         <v>33</v>
@@ -3254,10 +3254,10 @@
         <v>53</v>
       </c>
       <c r="E55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F55" t="s">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="G55" t="s">
         <v>6</v>
@@ -3274,7 +3274,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B56" t="s">
         <v>33</v>
@@ -3286,13 +3286,13 @@
         <v>44</v>
       </c>
       <c r="E56" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F56" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G56" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H56" t="s">
         <v>16</v>
@@ -3306,23 +3306,23 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C57" t="s">
         <v>48</v>
       </c>
       <c r="D57" t="s">
+        <v>114</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="G57" t="s">
         <v>6</v>
       </c>
@@ -3333,59 +3333,59 @@
         <v>17</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B58" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C58" t="s">
         <v>48</v>
       </c>
       <c r="D58" t="s">
+        <v>160</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="G58" t="s">
         <v>6</v>
       </c>
       <c r="H58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I58" t="s">
         <v>23</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C59" t="s">
         <v>12</v>
       </c>
       <c r="D59" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G59" t="s">
         <v>6</v>
@@ -3397,60 +3397,60 @@
         <v>23</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C60" t="s">
         <v>48</v>
       </c>
       <c r="D60" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G60" t="s">
         <v>6</v>
       </c>
       <c r="H60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I60" t="s">
         <v>23</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C61" t="s">
         <v>12</v>
       </c>
       <c r="D61" t="s">
+        <v>156</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="G61" t="s">
         <v>6</v>
       </c>
@@ -3461,27 +3461,27 @@
         <v>17</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C62" t="s">
         <v>52</v>
       </c>
       <c r="D62" t="s">
+        <v>119</v>
+      </c>
+      <c r="E62" t="s">
+        <v>120</v>
+      </c>
+      <c r="F62" t="s">
         <v>121</v>
-      </c>
-      <c r="E62" t="s">
-        <v>122</v>
-      </c>
-      <c r="F62" t="s">
-        <v>123</v>
       </c>
       <c r="G62" t="s">
         <v>6</v>
@@ -3498,22 +3498,22 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B63" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C63" t="s">
         <v>34</v>
       </c>
       <c r="D63" t="s">
+        <v>122</v>
+      </c>
+      <c r="E63" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" t="s">
         <v>124</v>
-      </c>
-      <c r="E63" t="s">
-        <v>125</v>
-      </c>
-      <c r="F63" t="s">
-        <v>126</v>
       </c>
       <c r="G63" t="s">
         <v>6</v>
@@ -3530,22 +3530,22 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B64" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C64" t="s">
         <v>52</v>
       </c>
       <c r="D64" t="s">
+        <v>122</v>
+      </c>
+      <c r="E64" t="s">
+        <v>123</v>
+      </c>
+      <c r="F64" t="s">
         <v>124</v>
-      </c>
-      <c r="E64" t="s">
-        <v>125</v>
-      </c>
-      <c r="F64" t="s">
-        <v>126</v>
       </c>
       <c r="G64" t="s">
         <v>6</v>
@@ -3562,22 +3562,22 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C65" t="s">
         <v>52</v>
       </c>
       <c r="D65" t="s">
+        <v>125</v>
+      </c>
+      <c r="E65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F65" t="s">
         <v>127</v>
-      </c>
-      <c r="E65" t="s">
-        <v>128</v>
-      </c>
-      <c r="F65" t="s">
-        <v>129</v>
       </c>
       <c r="G65" t="s">
         <v>6</v>
@@ -3594,22 +3594,22 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B66" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C66" t="s">
         <v>34</v>
       </c>
       <c r="D66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E66" t="s">
+        <v>126</v>
+      </c>
+      <c r="F66" t="s">
         <v>127</v>
-      </c>
-      <c r="E66" t="s">
-        <v>128</v>
-      </c>
-      <c r="F66" t="s">
-        <v>129</v>
       </c>
       <c r="G66" t="s">
         <v>6</v>
@@ -3626,22 +3626,22 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B67" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C67" t="s">
         <v>34</v>
       </c>
       <c r="D67" t="s">
+        <v>128</v>
+      </c>
+      <c r="E67" t="s">
+        <v>129</v>
+      </c>
+      <c r="F67" t="s">
         <v>130</v>
-      </c>
-      <c r="E67" t="s">
-        <v>131</v>
-      </c>
-      <c r="F67" t="s">
-        <v>132</v>
       </c>
       <c r="G67" t="s">
         <v>6</v>
@@ -3658,22 +3658,22 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B68" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C68" t="s">
         <v>52</v>
       </c>
       <c r="D68" t="s">
+        <v>128</v>
+      </c>
+      <c r="E68" t="s">
+        <v>129</v>
+      </c>
+      <c r="F68" t="s">
         <v>130</v>
-      </c>
-      <c r="E68" t="s">
-        <v>131</v>
-      </c>
-      <c r="F68" t="s">
-        <v>132</v>
       </c>
       <c r="G68" t="s">
         <v>6</v>
@@ -3690,22 +3690,22 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B69" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C69" t="s">
         <v>34</v>
       </c>
       <c r="D69" t="s">
+        <v>131</v>
+      </c>
+      <c r="E69" t="s">
+        <v>132</v>
+      </c>
+      <c r="F69" t="s">
         <v>133</v>
-      </c>
-      <c r="E69" t="s">
-        <v>134</v>
-      </c>
-      <c r="F69" t="s">
-        <v>135</v>
       </c>
       <c r="G69" t="s">
         <v>6</v>
@@ -3722,22 +3722,22 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B70" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C70" t="s">
         <v>52</v>
       </c>
       <c r="D70" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E70" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F70" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G70" t="s">
         <v>6</v>
@@ -3754,22 +3754,22 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B71" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C71" t="s">
         <v>34</v>
       </c>
       <c r="D71" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E71" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F71" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G71" t="s">
         <v>6</v>
@@ -3786,22 +3786,22 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B72" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C72" t="s">
         <v>52</v>
       </c>
       <c r="D72" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E72" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F72" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G72" t="s">
         <v>6</v>
@@ -3818,22 +3818,22 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B73" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C73" t="s">
         <v>34</v>
       </c>
       <c r="D73" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G73" t="s">
         <v>6</v>
@@ -3850,22 +3850,22 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B74" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C74" t="s">
         <v>34</v>
       </c>
       <c r="D74" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E74" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F74" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G74" t="s">
         <v>6</v>
@@ -3882,22 +3882,22 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B75" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C75" t="s">
         <v>52</v>
       </c>
       <c r="D75" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E75" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F75" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G75" t="s">
         <v>6</v>
@@ -3914,22 +3914,22 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C76" t="s">
         <v>52</v>
       </c>
       <c r="D76" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E76" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F76" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G76" t="s">
         <v>6</v>
@@ -3946,22 +3946,22 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B77" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C77" t="s">
         <v>48</v>
       </c>
       <c r="D77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E77" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F77" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G77" t="s">
         <v>6</v>
@@ -3978,22 +3978,22 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B78" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C78" t="s">
         <v>48</v>
       </c>
       <c r="D78" t="s">
+        <v>150</v>
+      </c>
+      <c r="E78" t="s">
+        <v>151</v>
+      </c>
+      <c r="F78" t="s">
         <v>152</v>
-      </c>
-      <c r="E78" t="s">
-        <v>153</v>
-      </c>
-      <c r="F78" t="s">
-        <v>154</v>
       </c>
       <c r="G78" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
In theory have subplot data with correct monitoring info (included added Mojave events) and correct plant info....so basically cleaned subplot data (but in theory I've had cleaned subplot data before lol)
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/04.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
+++ b/data/data-wrangling-intermediate/04.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BA4525C-4E4B-4CBD-9598-B01D4F601BC5}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE507DAB-981A-42A1-B3DE-7DE0A1F2F01B}"/>
   <bookViews>
-    <workbookView xWindow="41295" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1197,9 +1197,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1237,7 +1237,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1343,7 +1343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1485,7 +1485,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1496,8 +1496,8 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3234,7 +3234,7 @@
         <v>16</v>
       </c>
       <c r="I54" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="J54" t="s">
         <v>18</v>
@@ -3266,7 +3266,7 @@
         <v>16</v>
       </c>
       <c r="I55" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="J55" t="s">
         <v>18</v>

</xml_diff>